<commit_message>
week 1 of 2nd course
</commit_message>
<xml_diff>
--- a/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/W1_V2 3DFormulas.xlsx
+++ b/Visualization/Excel Specialization/Excel Skills for Business Intermediate I/Week 1/W1_V2 3DFormulas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nic\Documents\Freelance Training\Maquarie Uni\MOOCS\Course2\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\Excel Skills for Business Intermediate I\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBA55EB-1825-497E-811E-D9262A5FC3EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="43" windowWidth="37397" windowHeight="15994" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sean" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
     <definedName name="WeekEnding" localSheetId="1">Uma!$C$3</definedName>
     <definedName name="WeekEnding">Sean!$C$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -136,7 +137,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -507,15 +508,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Do Not Type" xfId="4"/>
+    <cellStyle name="Do Not Type" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="9" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input Custom" xfId="2"/>
-    <cellStyle name="Instructions" xfId="5"/>
+    <cellStyle name="Input Custom" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Instructions" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Table Totals" xfId="3"/>
+    <cellStyle name="Table Totals" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="3">
@@ -566,7 +567,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Expense Report" defaultPivotStyle="PivotStyleLight15">
-    <tableStyle name="Expense Report" pivot="0" count="3">
+    <tableStyle name="Expense Report" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="2"/>
       <tableStyleElement type="totalRow" dxfId="1"/>
       <tableStyleElement type="lastColumn" dxfId="0"/>
@@ -892,7 +893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="3"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -903,16 +904,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" customWidth="1"/>
-    <col min="8" max="11" width="9.453125"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" customWidth="1"/>
+    <col min="8" max="11" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
@@ -924,8 +925,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -933,7 +934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -941,7 +942,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -958,7 +959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -979,7 +980,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>412.72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1019,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1056,7 +1057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1071,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1091,14 +1092,14 @@
         <v>1143.1199999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1108,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>68.67</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1162,7 @@
         <v>145.80000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1182,14 +1183,14 @@
         <v>909.47</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1198,7 +1199,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>158.96</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1226,7 +1227,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -1271,14 +1272,14 @@
         <v>2848.96</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -1299,14 +1300,14 @@
         <v>4901.55</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -1321,7 +1322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1332,16 +1333,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
@@ -1353,8 +1354,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1498,14 +1499,14 @@
         <v>375</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1514,7 +1515,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>248.95</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1585,14 +1586,14 @@
         <v>248.95</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1602,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>86.64</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>165.1</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1649,7 +1650,7 @@
         <v>227.70000000000002</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -1682,14 +1683,14 @@
         <v>479.44000000000005</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -1710,14 +1711,14 @@
         <v>1103.3900000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -1732,7 +1733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="6"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
@@ -1743,16 +1744,16 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
@@ -1764,8 +1765,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>21</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1820,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1840,7 +1841,7 @@
         <v>739.68000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
@@ -1870,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>29.38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1910,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -1931,14 +1932,14 @@
         <v>919.06000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -1947,7 +1948,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>349.56</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
@@ -2018,14 +2019,14 @@
         <v>349.56</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -2034,7 +2035,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>268.79999999999995</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
@@ -2090,7 +2091,7 @@
         <v>85.48</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
@@ -2111,14 +2112,14 @@
         <v>354.28</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
@@ -2139,14 +2140,14 @@
         <v>1622.9</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2161,27 +2162,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="17.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.453125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="2.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="17.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="54.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>31</v>
       </c>
@@ -2193,8 +2194,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="12" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>14</v>
       </c>
@@ -2210,7 +2211,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
@@ -2227,119 +2228,182 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="5">
+        <f>SUM(Sean:Carlos!C7)</f>
+        <v>540</v>
+      </c>
+      <c r="D7" s="5">
+        <f>SUM(Sean:Carlos!D7)</f>
+        <v>528</v>
+      </c>
+      <c r="E7" s="5">
+        <f>SUM(Sean:Carlos!E7)</f>
+        <v>652</v>
+      </c>
       <c r="F7" s="22">
         <f t="shared" ref="F7:F13" si="0">SUM(C7:E7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="5">
+        <f>SUM(Sean:Carlos!C8)</f>
+        <v>361.8</v>
+      </c>
+      <c r="D8" s="5">
+        <f>SUM(Sean:Carlos!D8)</f>
+        <v>353.76</v>
+      </c>
+      <c r="E8" s="5">
+        <f>SUM(Sean:Carlos!E8)</f>
+        <v>436.84000000000003</v>
+      </c>
       <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1152.4000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="5">
+        <f>SUM(Sean:Carlos!C9)</f>
+        <v>83</v>
+      </c>
+      <c r="D9" s="5">
+        <f>SUM(Sean:Carlos!D9)</f>
+        <v>76.400000000000006</v>
+      </c>
+      <c r="E9" s="5">
+        <f>SUM(Sean:Carlos!E9)</f>
+        <v>83</v>
+      </c>
       <c r="F9" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>242.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="5">
+        <f>SUM(Sean:Carlos!C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <f>SUM(Sean:Carlos!D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <f>SUM(Sean:Carlos!E10)</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="5">
+        <f>SUM(Sean:Carlos!C11)</f>
+        <v>23.43</v>
+      </c>
+      <c r="D11" s="5">
+        <f>SUM(Sean:Carlos!D11)</f>
+        <v>78</v>
+      </c>
+      <c r="E11" s="5">
+        <f>SUM(Sean:Carlos!E11)</f>
+        <v>5.95</v>
+      </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>107.38000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="5">
+        <f>SUM(Sean:Carlos!C12)</f>
+        <v>125</v>
+      </c>
+      <c r="D12" s="5">
+        <f>SUM(Sean:Carlos!D12)</f>
+        <v>125</v>
+      </c>
+      <c r="E12" s="5">
+        <f>SUM(Sean:Carlos!E12)</f>
+        <v>125</v>
+      </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="5">
+        <f>SUM(Sean:Carlos!C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <f>SUM(Sean:Carlos!D13)</f>
+        <v>560</v>
+      </c>
+      <c r="E13" s="5">
+        <f>SUM(Sean:Carlos!E13)</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="11">
         <f>SUM(C8:C13)</f>
-        <v>0</v>
+        <v>593.23</v>
       </c>
       <c r="D14" s="11">
         <f t="shared" ref="D14:F14" si="1">SUM(D8:D13)</f>
-        <v>0</v>
+        <v>1193.1599999999999</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>650.79000000000008</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2437.1800000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
@@ -2348,83 +2412,119 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="14">
+        <f>SUM(Sean:Carlos!C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="14">
+        <f>SUM(Sean:Carlos!D17)</f>
+        <v>695</v>
+      </c>
+      <c r="E17" s="14">
+        <f>SUM(Sean:Carlos!E17)</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="9">
         <f t="shared" ref="F17:F20" si="2">SUM(C17:E17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="C18" s="14">
+        <f>SUM(Sean:Carlos!C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="14">
+        <f>SUM(Sean:Carlos!D18)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="14">
+        <f>SUM(Sean:Carlos!E18)</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="C19" s="14">
+        <f>SUM(Sean:Carlos!C19)</f>
+        <v>349.56</v>
+      </c>
+      <c r="D19" s="14">
+        <f>SUM(Sean:Carlos!D19)</f>
+        <v>68.67</v>
+      </c>
+      <c r="E19" s="14">
+        <f>SUM(Sean:Carlos!E19)</f>
+        <v>248.95</v>
+      </c>
       <c r="F19" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>667.18000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="C20" s="14">
+        <f>SUM(Sean:Carlos!C20)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="14">
+        <f>SUM(Sean:Carlos!D20)</f>
+        <v>145.80000000000001</v>
+      </c>
+      <c r="E20" s="14">
+        <f>SUM(Sean:Carlos!E20)</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>145.80000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="11">
         <f>SUM(C17:C20)</f>
-        <v>0</v>
+        <v>349.56</v>
       </c>
       <c r="D21" s="11">
         <f>SUM(D17:D20)</f>
-        <v>0</v>
+        <v>909.47</v>
       </c>
       <c r="E21" s="11">
         <f>SUM(E17:E20)</f>
-        <v>0</v>
+        <v>248.95</v>
       </c>
       <c r="F21" s="11">
         <f>SUM(F17:F20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1507.98</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
@@ -2433,111 +2533,147 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="C24" s="14">
+        <f>SUM(Sean:Carlos!C24)</f>
+        <v>158.96</v>
+      </c>
+      <c r="D24" s="14">
+        <f>SUM(Sean:Carlos!D24)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="14">
+        <f>SUM(Sean:Carlos!E24)</f>
+        <v>86.64</v>
+      </c>
       <c r="F24" s="9">
         <f t="shared" ref="F24:F27" si="3">SUM(C24:E24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>245.60000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="C25" s="14">
+        <f>SUM(Sean:Carlos!C25)</f>
+        <v>2690</v>
+      </c>
+      <c r="D25" s="14">
+        <f>SUM(Sean:Carlos!D25)</f>
+        <v>52.33</v>
+      </c>
+      <c r="E25" s="14">
+        <f>SUM(Sean:Carlos!E25)</f>
+        <v>112.77</v>
+      </c>
       <c r="F25" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2855.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="C26" s="14">
+        <f>SUM(Sean:Carlos!C26)</f>
+        <v>165.5</v>
+      </c>
+      <c r="D26" s="14">
+        <f>SUM(Sean:Carlos!D26)</f>
+        <v>165.5</v>
+      </c>
+      <c r="E26" s="14">
+        <f>SUM(Sean:Carlos!E26)</f>
+        <v>165.5</v>
+      </c>
       <c r="F26" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>496.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="C27" s="14">
+        <f>SUM(Sean:Carlos!C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="14">
+        <f>SUM(Sean:Carlos!D27)</f>
+        <v>85.48</v>
+      </c>
+      <c r="E27" s="14">
+        <f>SUM(Sean:Carlos!E27)</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85.48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="11">
         <f>SUM(C24:C27)</f>
-        <v>0</v>
+        <v>3014.46</v>
       </c>
       <c r="D28" s="11">
         <f>SUM(D24:D27)</f>
-        <v>0</v>
+        <v>303.31</v>
       </c>
       <c r="E28" s="11">
         <f>SUM(E24:E27)</f>
-        <v>0</v>
+        <v>364.90999999999997</v>
       </c>
       <c r="F28" s="11">
         <f>SUM(F24:F27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3682.68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="17">
         <f>SUM(C14,C21,C28)</f>
-        <v>0</v>
+        <v>3957.25</v>
       </c>
       <c r="D30" s="17">
         <f>SUM(D14,D21,D28)</f>
-        <v>0</v>
+        <v>2405.94</v>
       </c>
       <c r="E30" s="17">
         <f>SUM(E14,E21,E28)</f>
-        <v>0</v>
+        <v>1264.6500000000001</v>
       </c>
       <c r="F30" s="17">
         <f>SUM(F14,F21,F28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7627.84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>

</xml_diff>